<commit_message>
scaled data experiment added to bench mark dataset
</commit_message>
<xml_diff>
--- a/Experiments/BenchmarkDataset-syntetic/error.xlsx
+++ b/Experiments/BenchmarkDataset-syntetic/error.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkPlace\github projects\POCS_CLUSTERING\Experiments\BenchmarkDataset-syntetic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417B64FE-61FF-43B9-A69D-660FD6170186}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B45C7D-E614-4FF8-916E-77041BCB1368}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FDB4716B-F29C-493D-8FB8-1547E8985586}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{FDB4716B-F29C-493D-8FB8-1547E8985586}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="scaled" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="11">
   <si>
     <t>Flame</t>
   </si>
@@ -71,8 +73,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="172" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -109,12 +113,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -724,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1F213E-C3A1-4E6F-AC84-B5A536B3B68A}">
   <dimension ref="D4:W22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,16 +793,16 @@
       <c r="D5" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="4">
         <v>786.64737983553505</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="4">
         <v>772.60041264071401</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="4">
         <v>795.99491546698903</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="4">
         <v>798.90549933089096</v>
       </c>
       <c r="K5" t="s">
@@ -835,16 +848,16 @@
       <c r="D6" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="4">
         <v>225.17705712246601</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="4">
         <v>270.02067803419902</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="4">
         <v>270.11752732938902</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="4">
         <v>227.00514514091199</v>
       </c>
       <c r="K6" t="s">
@@ -890,16 +903,16 @@
       <c r="D7" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="4">
         <v>2713.4813512474798</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="4">
         <v>2804.4348742634402</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="4">
         <v>2806.3199960511101</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="4">
         <v>2778.8914383196202</v>
       </c>
       <c r="K7" t="s">
@@ -945,16 +958,16 @@
       <c r="D8" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="4">
         <v>5376840.7068671398</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="4">
         <v>6019760.2423958899</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="4">
         <v>5725605.5928340796</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="4">
         <v>5797087.3313369099</v>
       </c>
       <c r="K8" t="s">
@@ -1000,16 +1013,16 @@
       <c r="D9" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="4">
         <v>9275677.7878021505</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="4">
         <v>11662602.1520376</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="4">
         <v>9765588.7209774498</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="4">
         <v>9195646.6967367698</v>
       </c>
       <c r="K9" t="s">
@@ -1055,16 +1068,16 @@
       <c r="D10" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="4">
         <v>169389910.26341099</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="4">
         <v>194240587.607811</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="4">
         <v>170287976.135894</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="4">
         <v>170528882.32528901</v>
       </c>
       <c r="K10" t="s">
@@ -1110,16 +1123,16 @@
       <c r="D11" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="4">
         <v>207130701.25257099</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="4">
         <v>215479455.646294</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="4">
         <v>208323346.21015701</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="4">
         <v>208576752.75078699</v>
       </c>
       <c r="K11" t="s">
@@ -1203,16 +1216,16 @@
       <c r="D16" t="s">
         <v>0</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="4">
         <v>0.58294493655731605</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="4">
         <v>1.34245875385933E-4</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="4">
         <v>1.0458072055595699E-5</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="4">
         <v>4.0273741628689104</v>
       </c>
       <c r="K16" t="s">
@@ -1258,16 +1271,16 @@
       <c r="D17" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="4">
         <v>1.01684598917008E-13</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="4">
         <v>96.312369062867603</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="4">
         <v>2.9011337502570099E-3</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="4">
         <v>0.55501028209539804</v>
       </c>
       <c r="K17" t="s">
@@ -1313,16 +1326,16 @@
       <c r="D18" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="4">
         <v>0.137706652269143</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="4">
         <v>82.725797758038397</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="4">
         <v>2.3482490090578798E-10</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="4">
         <v>3.0715099031534301</v>
       </c>
       <c r="K18" t="s">
@@ -1368,16 +1381,16 @@
       <c r="D19" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="4">
         <v>7.1578554396051901</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="4">
         <v>362074.50197956403</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="4">
         <v>7.3686392772393203E-9</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="4">
         <v>4062.74052026248</v>
       </c>
       <c r="K19" t="s">
@@ -1423,16 +1436,16 @@
       <c r="D20" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="4">
         <v>166881.69548208901</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="4">
         <v>415852.59560611099</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="4">
         <v>1.33669936046072E-8</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="4">
         <v>2492.7476983250999</v>
       </c>
       <c r="K20" t="s">
@@ -1478,16 +1491,16 @@
       <c r="D21" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="4">
         <v>4.7112183889420903E-7</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="4">
         <v>20458023.513185099</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="4">
         <v>1.60213471123166E-7</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="4">
         <v>204571.38727944801</v>
       </c>
       <c r="K21" t="s">
@@ -1533,16 +1546,16 @@
       <c r="D22" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="4">
         <v>9618.6196344630298</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="4">
         <v>12968034.009276301</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="4">
         <v>2.9457602007750399E-7</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="4">
         <v>162298.43596849099</v>
       </c>
       <c r="K22" t="s">
@@ -1582,6 +1595,586 @@
       <c r="W22" s="2">
         <f t="shared" si="9"/>
         <v>1.2515269149694979E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29B21AB-07D9-430E-BF7E-A89849963638}">
+  <dimension ref="D5:H23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17:G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>58.035285728738202</v>
+      </c>
+      <c r="F6" s="1">
+        <v>56.831415149161799</v>
+      </c>
+      <c r="G6" s="1">
+        <v>58.875647789227898</v>
+      </c>
+      <c r="H6" s="1">
+        <v>58.9322841695124</v>
+      </c>
+    </row>
+    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>16.341400075997502</v>
+      </c>
+      <c r="F7" s="1">
+        <v>19.594764116634099</v>
+      </c>
+      <c r="G7" s="1">
+        <v>16.422733885414001</v>
+      </c>
+      <c r="H7" s="1">
+        <v>16.4737136083364</v>
+      </c>
+    </row>
+    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>92.703107130646501</v>
+      </c>
+      <c r="F8" s="1">
+        <v>94.302239819285404</v>
+      </c>
+      <c r="G8" s="1">
+        <v>93.499678133169894</v>
+      </c>
+      <c r="H8" s="1">
+        <v>93.760353938408798</v>
+      </c>
+    </row>
+    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1">
+        <v>124.322877086933</v>
+      </c>
+      <c r="F9" s="1">
+        <v>135.44624616752</v>
+      </c>
+      <c r="G9" s="1">
+        <v>130.69881446408399</v>
+      </c>
+      <c r="H9" s="1">
+        <v>124.8178615568</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="1">
+        <v>176.04036709896101</v>
+      </c>
+      <c r="F10" s="1">
+        <v>225.21898101160301</v>
+      </c>
+      <c r="G10" s="1">
+        <v>181.88203616916999</v>
+      </c>
+      <c r="H10" s="1">
+        <v>190.215708199582</v>
+      </c>
+    </row>
+    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1">
+        <v>181.96657410812199</v>
+      </c>
+      <c r="F11" s="1">
+        <v>212.29857602181099</v>
+      </c>
+      <c r="G11" s="1">
+        <v>182.90023964228001</v>
+      </c>
+      <c r="H11" s="1">
+        <v>183.162486937024</v>
+      </c>
+    </row>
+    <row r="12" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="1">
+        <v>219.604933570356</v>
+      </c>
+      <c r="F12" s="1">
+        <v>228.38504638984301</v>
+      </c>
+      <c r="G12" s="1">
+        <v>220.92389780705599</v>
+      </c>
+      <c r="H12" s="1">
+        <v>221.170941658359</v>
+      </c>
+    </row>
+    <row r="13" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1.4120366182701001E-2</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1.43620150332666E-7</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1.2230168925177E-6</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.27832868261004401</v>
+      </c>
+    </row>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3">
+        <v>7.3670638845611696E-15</v>
+      </c>
+      <c r="F18" s="1">
+        <v>6.9933482735851404</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1.6898056024502101E-12</v>
+      </c>
+      <c r="H18" s="1">
+        <v>4.0342457763853999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.15168434457879301</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1.9272779084060601</v>
+      </c>
+      <c r="G19" s="3">
+        <v>2.4627089119123299E-9</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0.32263606506494102</v>
+      </c>
+    </row>
+    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="1">
+        <v>7.9476195752089009E-3</v>
+      </c>
+      <c r="F20" s="1">
+        <v>5.0635204658864197</v>
+      </c>
+      <c r="G20" s="3">
+        <v>1.5467945746995999E-5</v>
+      </c>
+      <c r="H20" s="1">
+        <v>6.2347743870833E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1.6822812944005401</v>
+      </c>
+      <c r="F21" s="1">
+        <v>15.5207020989738</v>
+      </c>
+      <c r="G21" s="3">
+        <v>2.25621552870639E-8</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.164445495565991</v>
+      </c>
+    </row>
+    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="1">
+        <v>2.5104393678279098E-3</v>
+      </c>
+      <c r="F22" s="1">
+        <v>29.081187556379799</v>
+      </c>
+      <c r="G22" s="3">
+        <v>9.8978953629924606E-9</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.21630945857853601</v>
+      </c>
+    </row>
+    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2.2766050773005398E-3</v>
+      </c>
+      <c r="F23" s="1">
+        <v>13.617324184597599</v>
+      </c>
+      <c r="G23" s="3">
+        <v>8.5744346983787903E-7</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.22514271938208999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A267452F-F070-4967-B9EB-3C50F6D0FA1D}">
+  <dimension ref="C5:G23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>58.035285728738202</v>
+      </c>
+      <c r="E6" s="4">
+        <v>56.831415149161799</v>
+      </c>
+      <c r="F6" s="4">
+        <v>58.875647789227898</v>
+      </c>
+      <c r="G6" s="4">
+        <v>58.9322841695124</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4">
+        <v>16.341400075997502</v>
+      </c>
+      <c r="E7" s="4">
+        <v>19.594764116634099</v>
+      </c>
+      <c r="F7" s="4">
+        <v>16.422733885414001</v>
+      </c>
+      <c r="G7" s="4">
+        <v>16.4737136083364</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>92.703107130646501</v>
+      </c>
+      <c r="E8" s="4">
+        <v>94.302239819285404</v>
+      </c>
+      <c r="F8" s="4">
+        <v>93.499678133169894</v>
+      </c>
+      <c r="G8" s="4">
+        <v>93.760353938408798</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4">
+        <v>124.322877086933</v>
+      </c>
+      <c r="E9" s="4">
+        <v>135.44624616752</v>
+      </c>
+      <c r="F9" s="4">
+        <v>130.69881446408399</v>
+      </c>
+      <c r="G9" s="4">
+        <v>124.8178615568</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="4">
+        <v>176.04036709896101</v>
+      </c>
+      <c r="E10" s="4">
+        <v>225.21898101160301</v>
+      </c>
+      <c r="F10" s="4">
+        <v>181.88203616916999</v>
+      </c>
+      <c r="G10" s="4">
+        <v>190.215708199582</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="4">
+        <v>181.96657410812199</v>
+      </c>
+      <c r="E11" s="4">
+        <v>212.29857602181099</v>
+      </c>
+      <c r="F11" s="4">
+        <v>182.90023964228001</v>
+      </c>
+      <c r="G11" s="4">
+        <v>183.162486937024</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="4">
+        <v>219.604933570356</v>
+      </c>
+      <c r="E12" s="4">
+        <v>228.38504638984301</v>
+      </c>
+      <c r="F12" s="4">
+        <v>220.92389780705599</v>
+      </c>
+      <c r="G12" s="4">
+        <v>221.170941658359</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1.4120366182701001E-2</v>
+      </c>
+      <c r="E17" s="5">
+        <v>1.43620150332666E-7</v>
+      </c>
+      <c r="F17" s="5">
+        <v>1.2230168925177E-6</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0.27832868261004401</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="5">
+        <v>7.3670638845611696E-15</v>
+      </c>
+      <c r="E18" s="5">
+        <v>6.9933482735851404</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1.6898056024502101E-12</v>
+      </c>
+      <c r="G18" s="5">
+        <v>4.0342457763853999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0.15168434457879301</v>
+      </c>
+      <c r="E19" s="5">
+        <v>1.9272779084060601</v>
+      </c>
+      <c r="F19" s="5">
+        <v>2.4627089119123299E-9</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0.32263606506494102</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="5">
+        <v>7.9476195752089009E-3</v>
+      </c>
+      <c r="E20" s="5">
+        <v>5.0635204658864197</v>
+      </c>
+      <c r="F20" s="5">
+        <v>1.5467945746995999E-5</v>
+      </c>
+      <c r="G20" s="5">
+        <v>6.2347743870833E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1.6822812944005401</v>
+      </c>
+      <c r="E21" s="5">
+        <v>15.5207020989738</v>
+      </c>
+      <c r="F21" s="5">
+        <v>2.25621552870639E-8</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0.164445495565991</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="5">
+        <v>2.5104393678279098E-3</v>
+      </c>
+      <c r="E22" s="5">
+        <v>29.081187556379799</v>
+      </c>
+      <c r="F22" s="5">
+        <v>9.8978953629924606E-9</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0.21630945857853601</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="5">
+        <v>2.2766050773005398E-3</v>
+      </c>
+      <c r="E23" s="5">
+        <v>13.617324184597599</v>
+      </c>
+      <c r="F23" s="5">
+        <v>8.5744346983787903E-7</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0.22514271938208999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>